<commit_message>
Bunch of updates. Fixed issues with login and logout.
</commit_message>
<xml_diff>
--- a/Elantech Assistant DB/DB Layout.xlsx
+++ b/Elantech Assistant DB/DB Layout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25225"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kingg\Documents\GitHub\Elantech-Inventory-Management\Elantech Assistant DB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giuseppe\Documents\GitHub\Elantech-Assistant\Elantech Assistant DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9663A8F7-6FF2-4BA8-9181-5123B5E42E1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B66052D-5469-48BD-A422-010EC1008EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="5025" windowWidth="5625" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="30750" yWindow="2895" windowWidth="7185" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="58">
   <si>
     <t>Product Information</t>
   </si>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Condition Upon Delivery</t>
-  </si>
-  <si>
-    <t>Does PO Number Get Duplicated?</t>
   </si>
   <si>
     <t>Outgoing Orders</t>
@@ -536,10 +533,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D50"/>
+  <dimension ref="A1:B50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="A17" sqref="A17:A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,7 +546,7 @@
     <col min="4" max="4" width="31.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,7 +554,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -565,7 +562,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -573,7 +570,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -581,7 +578,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -589,7 +586,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -597,7 +594,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -605,12 +602,12 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -618,18 +615,15 @@
         <v>47</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
         <v>42</v>
       </c>
-      <c r="D10" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -637,7 +631,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -645,7 +639,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -653,7 +647,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>25</v>
       </c>
@@ -661,7 +655,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
         <v>11</v>
       </c>
@@ -676,7 +670,7 @@
         <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -692,7 +686,7 @@
         <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -700,7 +694,7 @@
         <v>15</v>
       </c>
       <c r="B21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -708,7 +702,7 @@
         <v>16</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -716,7 +710,7 @@
         <v>17</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -724,7 +718,7 @@
         <v>18</v>
       </c>
       <c r="B24" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -732,7 +726,7 @@
         <v>19</v>
       </c>
       <c r="B25" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -745,7 +739,7 @@
         <v>21</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -886,7 +880,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1">
         <v>40</v>

</xml_diff>